<commit_message>
added VAR updated and graphs
</commit_message>
<xml_diff>
--- a/final_sets/VARallyrs.xlsx
+++ b/final_sets/VARallyrs.xlsx
@@ -1263,6 +1263,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1348,10 +1349,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C428"/>
+  <dimension ref="A2:C427"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A412" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C428" activeCellId="0" sqref="C428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4762,11 +4763,6 @@
       </c>
       <c r="C427" s="0" t="n">
         <v>-0.0404985162793441</v>
-      </c>
-    </row>
-    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C428" s="0" t="n">
-        <v>-0.031358324704937</v>
       </c>
     </row>
   </sheetData>
@@ -4785,10 +4781,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C428"/>
+  <dimension ref="A2:C427"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A413" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C428" activeCellId="0" sqref="C428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -8201,15 +8197,10 @@
         <v>-0.0339890511984751</v>
       </c>
     </row>
-    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C428" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -8222,10 +8213,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C428"/>
+  <dimension ref="A2:C427"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A410" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G410" activeCellId="0" sqref="G410"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -11638,15 +11629,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C428" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -11659,10 +11645,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C428"/>
+  <dimension ref="A2:C427"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A415" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A428" activeCellId="0" sqref="A428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -15075,15 +15061,10 @@
         <v>-0.053282201959581</v>
       </c>
     </row>
-    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C428" s="0" t="n">
-        <v>-0.0323164830595298</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -15096,10 +15077,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C428"/>
+  <dimension ref="A2:C427"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A421" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C428" activeCellId="0" sqref="C428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -18512,15 +18493,10 @@
         <v>-0.0681688627181854</v>
       </c>
     </row>
-    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C428" s="0" t="n">
-        <v>-0.0367112212185169</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -18533,10 +18509,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C428"/>
+  <dimension ref="A2:C427"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A426" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C428" activeCellId="0" sqref="C428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -21949,15 +21925,10 @@
         <v>-0.0524106904645146</v>
       </c>
     </row>
-    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C428" s="0" t="n">
-        <v>-0.02891116618913</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -21970,10 +21941,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C428"/>
+  <dimension ref="A2:C427"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A407" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C428" activeCellId="0" sqref="C428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -25386,15 +25357,10 @@
         <v>-0.0659266519749825</v>
       </c>
     </row>
-    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C428" s="0" t="n">
-        <v>-0.0548993069702122</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -25407,10 +25373,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C428"/>
+  <dimension ref="A2:C427"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A419" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C428" activeCellId="0" sqref="C428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -28823,15 +28789,10 @@
         <v>-0.0671566645515839</v>
       </c>
     </row>
-    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C428" s="0" t="n">
-        <v>-0.0640255524345336</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -28844,10 +28805,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C428"/>
+  <dimension ref="A2:C427"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A418" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C428" activeCellId="0" sqref="C428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -32260,15 +32221,10 @@
         <v>-0.0403532984080643</v>
       </c>
     </row>
-    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C428" s="0" t="n">
-        <v>-0.0317711699115411</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -32281,10 +32237,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C428"/>
+  <dimension ref="A2:C427"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A415" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C428" activeCellId="0" sqref="C428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -35697,15 +35653,10 @@
         <v>-0.0524138277149114</v>
       </c>
     </row>
-    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C428" s="0" t="n">
-        <v>-0.0206942696244376</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -35718,10 +35669,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C428"/>
+  <dimension ref="A2:C427"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A418" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C428" activeCellId="0" sqref="C428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -39134,15 +39085,10 @@
         <v>-0.067100125877347</v>
       </c>
     </row>
-    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C428" s="0" t="n">
-        <v>-0.0203166976478476</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>